<commit_message>
Update and fix batch spreadsheets
</commit_message>
<xml_diff>
--- a/data/fractionation/221012 Batch 126 Summary Water Yr.xlsx
+++ b/data/fractionation/221012 Batch 126 Summary Water Yr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\SIP Pipeline\Mike\221012 Batch 126 PNNL and water yr repeat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Banfield\WaterYear\SIP\data\fractionation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235E25EB-4EC4-4170-A607-F2F33DD314E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640C553C-D74B-4597-992A-47D41E37CEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="622" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-21710" windowWidth="38620" windowHeight="21100" tabRatio="622" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table of Contents" sheetId="22" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1220" uniqueCount="202">
   <si>
     <t>calculated density p(20)</t>
   </si>
@@ -741,9 +741,6 @@
   </si>
   <si>
     <t>J</t>
-  </si>
-  <si>
-    <t>K</t>
   </si>
   <si>
     <t>Isotope</t>
@@ -875,6 +872,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -954,7 +952,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1077,21 +1075,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1244,11 +1233,6 @@
     </xf>
     <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="16" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="16" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1263,15 +1247,11 @@
     <xf numFmtId="165" fontId="16" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="16" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1291,24 +1271,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="22" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1319,6 +1281,18 @@
     </xf>
     <xf numFmtId="165" fontId="22" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="22" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1533,7 +1507,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Summary!$C$6:$C$24</c:f>
+              <c:f>Summary!$C$5:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1599,7 +1573,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$D$6:$D$24</c:f>
+              <c:f>Summary!$D$5:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1708,7 +1682,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Summary!$F$6:$F$24</c:f>
+              <c:f>Summary!$F$5:$F$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1774,7 +1748,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$G$6:$G$24</c:f>
+              <c:f>Summary!$G$5:$G$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -2299,7 +2273,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Summary!$A$5:$A$26</c:f>
+              <c:f>Summary!$A$4:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
@@ -2374,7 +2348,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$C$5:$C$26</c:f>
+              <c:f>Summary!$C$4:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="22"/>
@@ -2486,7 +2460,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Summary!$A$5:$A$26</c:f>
+              <c:f>Summary!$A$4:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
@@ -2561,7 +2535,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$F$5:$F$26</c:f>
+              <c:f>Summary!$F$4:$F$25</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="22"/>
@@ -4087,13 +4061,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>232833</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>16934</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>734482</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>82549</xdr:rowOff>
@@ -4125,13 +4099,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>260349</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>88899</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>355600</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>122766</xdr:rowOff>
@@ -4565,19 +4539,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E138FBF1-D534-4F7E-950C-764D2E6B8C19}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.7"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="11.29296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.703125" customWidth="1"/>
-    <col min="4" max="4" width="17.29296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.52734375" customWidth="1"/>
-    <col min="7" max="7" width="18.703125" customWidth="1"/>
+    <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" customWidth="1"/>
+    <col min="4" max="4" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" customWidth="1"/>
+    <col min="7" max="7" width="18.7265625" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
   </cols>
@@ -4587,7 +4561,7 @@
         <v>183</v>
       </c>
       <c r="B1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -4595,7 +4569,7 @@
         <v>184</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4615,16 +4589,16 @@
         <v>190</v>
       </c>
       <c r="F4" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="G4" s="27" t="s">
         <v>196</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>197</v>
       </c>
       <c r="H4" s="27" t="s">
         <v>191</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J4" s="27" t="s">
         <v>188</v>
@@ -4653,7 +4627,7 @@
         <v>3000</v>
       </c>
       <c r="H5" s="52">
-        <f>Summary!D27</f>
+        <f>Summary!D26</f>
         <v>49.08513751382133</v>
       </c>
       <c r="I5" s="52">
@@ -4683,7 +4657,7 @@
         <v>3000</v>
       </c>
       <c r="H6" s="52">
-        <f>Summary!G27</f>
+        <f>Summary!G26</f>
         <v>48.639814384326741</v>
       </c>
       <c r="I6" s="52">
@@ -4692,12 +4666,12 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -4713,9 +4687,9 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.7"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.35">
+    <row r="1" spans="1:13" ht="26">
       <c r="A1" s="32" t="s">
         <v>55</v>
       </c>
@@ -5330,9 +5304,9 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.7"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.35">
+    <row r="1" spans="1:13" ht="26">
       <c r="A1" s="32" t="s">
         <v>55</v>
       </c>
@@ -5947,9 +5921,9 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.7"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.35">
+    <row r="1" spans="1:13" ht="26">
       <c r="A1" s="32" t="s">
         <v>55</v>
       </c>
@@ -6563,9 +6537,9 @@
       <selection activeCell="D33" sqref="D32:D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.7"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.35">
+    <row r="1" spans="1:13" ht="26">
       <c r="A1" s="32" t="s">
         <v>55</v>
       </c>
@@ -7179,9 +7153,9 @@
       <selection activeCell="A2" sqref="A2:G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.7"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.35">
+    <row r="1" spans="1:13" ht="26">
       <c r="A1" s="32" t="s">
         <v>55</v>
       </c>
@@ -7707,9 +7681,9 @@
       <selection activeCell="A2" sqref="A2:G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.7"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.35">
+    <row r="1" spans="1:13" ht="26">
       <c r="A1" s="32" t="s">
         <v>55</v>
       </c>
@@ -8235,9 +8209,9 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.7"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.35">
+    <row r="1" spans="1:13" ht="26">
       <c r="A1" s="32" t="s">
         <v>55</v>
       </c>
@@ -8763,9 +8737,9 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.7"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.35">
+    <row r="1" spans="1:13" ht="26">
       <c r="A1" s="32" t="s">
         <v>55</v>
       </c>
@@ -10510,9 +10484,9 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.7"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.35">
+    <row r="1" spans="1:13" ht="26">
       <c r="A1" s="32" t="s">
         <v>55</v>
       </c>
@@ -11039,9 +11013,9 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.7"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.35">
+    <row r="1" spans="1:13" ht="26">
       <c r="A1" s="32" t="s">
         <v>55</v>
       </c>
@@ -12779,1195 +12753,719 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA4E3B1-5772-4D1F-AF5A-033072A123CA}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.87890625" defaultRowHeight="12.7"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="9.52734375" style="58" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.41015625" style="58" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.703125" style="58" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="10.87890625" style="58"/>
-    <col min="8" max="8" width="10.87890625" style="58" customWidth="1"/>
-    <col min="9" max="9" width="10.87890625" style="58"/>
-    <col min="10" max="11" width="11" style="58" customWidth="1"/>
-    <col min="12" max="16384" width="10.87890625" style="58"/>
+    <col min="1" max="1" width="9.54296875" style="58" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" style="58" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" style="58" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.90625" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13" thickBot="1">
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-    </row>
-    <row r="2" spans="1:13" ht="13" thickTop="1">
+    <row r="1" spans="1:7" ht="13" thickTop="1">
+      <c r="A1" s="64" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="98">
+        <f>'Tube Loading'!$F$37</f>
+        <v>1454</v>
+      </c>
+      <c r="C1" s="99" t="str">
+        <f>_xlfn.TEXTJOIN("-",TRUE,'Tube Loading'!$F$37,"density")</f>
+        <v>1454-density</v>
+      </c>
+      <c r="D1" s="100" t="str">
+        <f>_xlfn.TEXTJOIN("-",TRUE,'Tube Loading'!$F$37,"conc")</f>
+        <v>1454-conc</v>
+      </c>
+      <c r="E1" s="58">
+        <f>'Tube Loading'!$F$38</f>
+        <v>1469</v>
+      </c>
+      <c r="F1" s="58" t="str">
+        <f>_xlfn.TEXTJOIN("-",TRUE,'Tube Loading'!$F$38,"density")</f>
+        <v>1469-density</v>
+      </c>
+      <c r="G1" s="58" t="str">
+        <f>_xlfn.TEXTJOIN("-",TRUE,'Tube Loading'!$F$38,"conc")</f>
+        <v>1469-conc</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="64" t="s">
-        <v>178</v>
-      </c>
-      <c r="B2" s="95">
-        <f>'Tube Loading'!F37</f>
-        <v>1454</v>
-      </c>
-      <c r="C2" s="96"/>
+        <v>179</v>
+      </c>
+      <c r="B2" s="96" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" s="101"/>
       <c r="D2" s="97"/>
-      <c r="E2" s="95">
-        <f>'Tube Loading'!F38</f>
-        <v>1469</v>
-      </c>
-      <c r="F2" s="96"/>
+      <c r="E2" s="96" t="s">
+        <v>194</v>
+      </c>
+      <c r="F2" s="101"/>
       <c r="G2" s="97"/>
-      <c r="H2" s="95">
-        <f>'Tube Loading'!F39</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="96"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="95">
-        <f>'Tube Loading'!F40</f>
-        <v>0</v>
-      </c>
-      <c r="L2" s="96"/>
-      <c r="M2" s="97"/>
-    </row>
-    <row r="3" spans="1:13">
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="64" t="s">
-        <v>179</v>
-      </c>
-      <c r="B3" s="98" t="s">
-        <v>193</v>
-      </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="98" t="s">
-        <v>194</v>
-      </c>
-      <c r="F3" s="99"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="98" t="s">
-        <v>195</v>
-      </c>
-      <c r="I3" s="99"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="98" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="99"/>
-      <c r="M3" s="100"/>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="64" t="s">
         <v>168</v>
       </c>
-      <c r="B4" s="78" t="s">
+      <c r="B3" s="75" t="s">
         <v>180</v>
       </c>
-      <c r="C4" s="79" t="s">
+      <c r="C3" s="76" t="s">
         <v>181</v>
       </c>
-      <c r="D4" s="80" t="s">
+      <c r="D3" s="77" t="s">
         <v>169</v>
       </c>
-      <c r="E4" s="78" t="s">
+      <c r="E3" s="75" t="s">
         <v>180</v>
       </c>
-      <c r="F4" s="79" t="s">
+      <c r="F3" s="76" t="s">
         <v>181</v>
       </c>
-      <c r="G4" s="80" t="s">
+      <c r="G3" s="77" t="s">
         <v>169</v>
       </c>
-      <c r="H4" s="78" t="s">
-        <v>180</v>
-      </c>
-      <c r="I4" s="79" t="s">
-        <v>181</v>
-      </c>
-      <c r="J4" s="80" t="s">
-        <v>169</v>
-      </c>
-      <c r="K4" s="78" t="s">
-        <v>180</v>
-      </c>
-      <c r="L4" s="79" t="s">
-        <v>181</v>
-      </c>
-      <c r="M4" s="80" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="58">
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="58">
         <v>1</v>
       </c>
-      <c r="B5" s="68" t="str">
+      <c r="B4" s="68" t="str">
         <f>'Tube I'!G2</f>
         <v>A1</v>
       </c>
-      <c r="C5" s="69">
+      <c r="C4" s="69">
         <f>'Tube I'!F2</f>
         <v>1.7031812900000016</v>
       </c>
-      <c r="D5" s="70">
+      <c r="D4" s="70">
         <v>3.0638726191165099E-2</v>
       </c>
-      <c r="E5" s="68" t="str">
+      <c r="E4" s="68" t="str">
         <f>'Tube J'!G2</f>
         <v>G3</v>
       </c>
-      <c r="F5" s="69">
+      <c r="F4" s="69">
         <f>'Tube J'!F2</f>
         <v>1.7024709960000024</v>
       </c>
-      <c r="G5" s="70">
+      <c r="G4" s="70">
         <v>-3.3059099849863682E-3</v>
       </c>
-      <c r="H5" s="68" t="str">
-        <f>'Tube K'!G2</f>
-        <v>D6</v>
-      </c>
-      <c r="I5" s="69">
-        <f>'Tube K'!F2</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="J5" s="70"/>
-      <c r="K5" s="68" t="str">
-        <f>'Tube L'!G2</f>
-        <v>C9</v>
-      </c>
-      <c r="L5" s="69">
-        <f>'Tube L'!F2</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="M5" s="70"/>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="58">
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="58">
         <v>2</v>
       </c>
-      <c r="B6" s="71" t="str">
+      <c r="B5" s="71" t="str">
         <f>'Tube I'!G3</f>
         <v>B1</v>
       </c>
-      <c r="C6" s="72">
+      <c r="C5" s="72">
         <f>'Tube I'!F3</f>
         <v>1.7676541300000022</v>
       </c>
-      <c r="D6" s="73">
+      <c r="D5" s="73">
         <v>4.991602166654039E-2</v>
       </c>
-      <c r="E6" s="71" t="str">
+      <c r="E5" s="71" t="str">
         <f>'Tube J'!G3</f>
         <v>H3</v>
       </c>
-      <c r="F6" s="69">
+      <c r="F5" s="69">
         <f>'Tube J'!F3</f>
         <v>1.7680365960000017</v>
       </c>
-      <c r="G6" s="73">
+      <c r="G5" s="73">
         <v>-4.2326176684165549E-3</v>
       </c>
-      <c r="H6" s="71" t="str">
-        <f>'Tube K'!G3</f>
-        <v>C6</v>
-      </c>
-      <c r="I6" s="72">
-        <f>'Tube K'!F3</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="J6" s="73"/>
-      <c r="K6" s="71" t="str">
-        <f>'Tube L'!G3</f>
-        <v>D9</v>
-      </c>
-      <c r="L6" s="72">
-        <f>'Tube L'!F3</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="M6" s="73"/>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="58">
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="58">
         <v>3</v>
       </c>
-      <c r="B7" s="71" t="str">
+      <c r="B6" s="71" t="str">
         <f>'Tube I'!G4</f>
         <v>C1</v>
       </c>
-      <c r="C7" s="72">
+      <c r="C6" s="72">
         <f>'Tube I'!F4</f>
         <v>1.762190330000001</v>
       </c>
-      <c r="D7" s="73">
+      <c r="D6" s="73">
         <v>1.7295430091523938E-2</v>
       </c>
-      <c r="E7" s="71" t="str">
+      <c r="E6" s="71" t="str">
         <f>'Tube J'!G4</f>
         <v>H4</v>
       </c>
-      <c r="F7" s="69">
+      <c r="F6" s="69">
         <f>'Tube J'!F4</f>
         <v>1.7625727960000006</v>
       </c>
-      <c r="G7" s="73">
+      <c r="G6" s="73">
         <v>-5.587680700336232E-3</v>
       </c>
-      <c r="H7" s="71" t="str">
-        <f>'Tube K'!G4</f>
-        <v>B6</v>
-      </c>
-      <c r="I7" s="72">
-        <f>'Tube K'!F4</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="J7" s="73"/>
-      <c r="K7" s="71" t="str">
-        <f>'Tube L'!G4</f>
-        <v>E9</v>
-      </c>
-      <c r="L7" s="72">
-        <f>'Tube L'!F4</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="M7" s="73"/>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="58">
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="58">
         <v>4</v>
       </c>
-      <c r="B8" s="71" t="str">
+      <c r="B7" s="71" t="str">
         <f>'Tube I'!G5</f>
         <v>D1</v>
       </c>
-      <c r="C8" s="72">
+      <c r="C7" s="72">
         <f>'Tube I'!F5</f>
         <v>1.7556337700000011</v>
       </c>
-      <c r="D8" s="73">
+      <c r="D7" s="73">
         <v>1.2174888501875517E-2</v>
       </c>
-      <c r="E8" s="71" t="str">
+      <c r="E7" s="71" t="str">
         <f>'Tube J'!G5</f>
         <v>G4</v>
       </c>
-      <c r="F8" s="69">
+      <c r="F7" s="69">
         <f>'Tube J'!F5</f>
         <v>1.7560162360000007</v>
       </c>
-      <c r="G8" s="73">
+      <c r="G7" s="73">
         <v>-1.6628584043697658E-2</v>
       </c>
-      <c r="H8" s="71" t="str">
-        <f>'Tube K'!G5</f>
-        <v>A6</v>
-      </c>
-      <c r="I8" s="72">
-        <f>'Tube K'!F5</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="J8" s="73"/>
-      <c r="K8" s="71" t="str">
-        <f>'Tube L'!G5</f>
-        <v>F9</v>
-      </c>
-      <c r="L8" s="72">
-        <f>'Tube L'!F5</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="M8" s="73"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="58">
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="58">
         <v>5</v>
       </c>
-      <c r="B9" s="71" t="str">
+      <c r="B8" s="71" t="str">
         <f>'Tube I'!G6</f>
         <v>E1</v>
       </c>
-      <c r="C9" s="72">
+      <c r="C8" s="72">
         <f>'Tube I'!F6</f>
         <v>1.7490772100000029</v>
       </c>
-      <c r="D9" s="73">
+      <c r="D8" s="73">
         <v>1.7139137608311841E-2</v>
       </c>
-      <c r="E9" s="71" t="str">
+      <c r="E8" s="71" t="str">
         <f>'Tube J'!G6</f>
         <v>F4</v>
       </c>
-      <c r="F9" s="69">
+      <c r="F8" s="69">
         <f>'Tube J'!F6</f>
         <v>1.7494596760000025</v>
       </c>
-      <c r="G9" s="73">
+      <c r="G8" s="73">
         <v>0.10105949809818937</v>
       </c>
-      <c r="H9" s="71" t="str">
-        <f>'Tube K'!G6</f>
-        <v>A7</v>
-      </c>
-      <c r="I9" s="72">
-        <f>'Tube K'!F6</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="J9" s="73"/>
-      <c r="K9" s="71" t="str">
-        <f>'Tube L'!G6</f>
-        <v>G9</v>
-      </c>
-      <c r="L9" s="72">
-        <f>'Tube L'!F6</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="M9" s="73"/>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="58">
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="58">
         <v>6</v>
       </c>
-      <c r="B10" s="71" t="str">
+      <c r="B9" s="71" t="str">
         <f>'Tube I'!G7</f>
         <v>F1</v>
       </c>
-      <c r="C10" s="72">
+      <c r="C9" s="72">
         <f>'Tube I'!F7</f>
         <v>1.7425206500000012</v>
       </c>
-      <c r="D10" s="73">
+      <c r="D9" s="73">
         <v>1.2072853162397326</v>
       </c>
-      <c r="E10" s="71" t="str">
+      <c r="E9" s="71" t="str">
         <f>'Tube J'!G7</f>
         <v>E4</v>
       </c>
-      <c r="F10" s="69">
+      <c r="F9" s="69">
         <f>'Tube J'!F7</f>
         <v>1.7429031160000008</v>
       </c>
-      <c r="G10" s="73">
+      <c r="G9" s="73">
         <v>0.3705066669646786</v>
       </c>
-      <c r="H10" s="71" t="str">
-        <f>'Tube K'!G7</f>
-        <v>B7</v>
-      </c>
-      <c r="I10" s="72">
-        <f>'Tube K'!F7</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="J10" s="73"/>
-      <c r="K10" s="71" t="str">
-        <f>'Tube L'!G7</f>
-        <v>H9</v>
-      </c>
-      <c r="L10" s="72">
-        <f>'Tube L'!F7</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="M10" s="73"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="58">
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="58">
         <v>7</v>
       </c>
-      <c r="B11" s="101" t="str">
+      <c r="B10" s="90" t="str">
         <f>'Tube I'!G8</f>
         <v>G1</v>
       </c>
-      <c r="C11" s="102">
+      <c r="C10" s="91">
         <f>'Tube I'!F8</f>
         <v>1.7359640900000013</v>
       </c>
-      <c r="D11" s="103">
+      <c r="D10" s="92">
         <v>2.7173778273730442</v>
       </c>
-      <c r="E11" s="71" t="str">
+      <c r="E10" s="71" t="str">
         <f>'Tube J'!G8</f>
         <v>D4</v>
       </c>
-      <c r="F11" s="69">
+      <c r="F10" s="69">
         <f>'Tube J'!F8</f>
         <v>1.7363465560000009</v>
       </c>
-      <c r="G11" s="73">
+      <c r="G10" s="73">
         <v>0.77910944096039059</v>
       </c>
-      <c r="H11" s="71" t="str">
-        <f>'Tube K'!G8</f>
-        <v>C7</v>
-      </c>
-      <c r="I11" s="72">
-        <f>'Tube K'!F8</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="J11" s="73"/>
-      <c r="K11" s="71" t="str">
-        <f>'Tube L'!G8</f>
-        <v>H10</v>
-      </c>
-      <c r="L11" s="72">
-        <f>'Tube L'!F8</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="M11" s="74"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="58">
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="58">
         <v>8</v>
       </c>
-      <c r="B12" s="71" t="str">
+      <c r="B11" s="71" t="str">
         <f>'Tube I'!G9</f>
         <v>H1</v>
       </c>
-      <c r="C12" s="72">
+      <c r="C11" s="72">
         <f>'Tube I'!F9</f>
         <v>1.7305002900000019</v>
       </c>
-      <c r="D12" s="73">
+      <c r="D11" s="73">
         <v>3.9252857972637938</v>
       </c>
-      <c r="E12" s="71" t="str">
+      <c r="E11" s="71" t="str">
         <f>'Tube J'!G9</f>
         <v>C4</v>
       </c>
-      <c r="F12" s="69">
+      <c r="F11" s="69">
         <f>'Tube J'!F9</f>
         <v>1.7308827560000015</v>
       </c>
-      <c r="G12" s="73">
+      <c r="G11" s="73">
         <v>2.2353595488776281</v>
       </c>
-      <c r="H12" s="71" t="str">
-        <f>'Tube K'!G9</f>
-        <v>D7</v>
-      </c>
-      <c r="I12" s="72">
-        <f>'Tube K'!F9</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="J12" s="73"/>
-      <c r="K12" s="71" t="str">
-        <f>'Tube L'!G9</f>
-        <v>G10</v>
-      </c>
-      <c r="L12" s="72">
-        <f>'Tube L'!F9</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="M12" s="74"/>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="58">
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="58">
         <v>9</v>
       </c>
-      <c r="B13" s="71" t="str">
+      <c r="B12" s="71" t="str">
         <f>'Tube I'!G10</f>
         <v>H2</v>
       </c>
-      <c r="C13" s="72">
+      <c r="C12" s="72">
         <f>'Tube I'!F10</f>
         <v>1.7250364900000026</v>
       </c>
-      <c r="D13" s="73">
+      <c r="D12" s="73">
         <v>7.8811974146085264</v>
       </c>
-      <c r="E13" s="71" t="str">
+      <c r="E12" s="71" t="str">
         <f>'Tube J'!G10</f>
         <v>B4</v>
       </c>
-      <c r="F13" s="69">
+      <c r="F12" s="69">
         <f>'Tube J'!F10</f>
         <v>1.7243261960000034</v>
       </c>
-      <c r="G13" s="73">
+      <c r="G12" s="73">
         <v>7.253843311074113</v>
       </c>
-      <c r="H13" s="71" t="str">
-        <f>'Tube K'!G10</f>
-        <v>E7</v>
-      </c>
-      <c r="I13" s="72">
-        <f>'Tube K'!F10</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="J13" s="73"/>
-      <c r="K13" s="71" t="str">
-        <f>'Tube L'!G10</f>
-        <v>F10</v>
-      </c>
-      <c r="L13" s="72">
-        <f>'Tube L'!F10</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="M13" s="74"/>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="58">
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="58">
         <v>10</v>
       </c>
-      <c r="B14" s="101" t="str">
+      <c r="B13" s="90" t="str">
         <f>'Tube I'!G11</f>
         <v>G2</v>
       </c>
-      <c r="C14" s="102">
+      <c r="C13" s="91">
         <f>'Tube I'!F11</f>
         <v>1.7184799300000009</v>
       </c>
-      <c r="D14" s="103">
+      <c r="D13" s="92">
         <v>8.8030325626338506</v>
       </c>
-      <c r="E14" s="71" t="str">
+      <c r="E13" s="71" t="str">
         <f>'Tube J'!G11</f>
         <v>A4</v>
       </c>
-      <c r="F14" s="69">
+      <c r="F13" s="69">
         <f>'Tube J'!F11</f>
         <v>1.7188623960000005</v>
       </c>
-      <c r="G14" s="73">
+      <c r="G13" s="73">
         <v>10.274040336575727</v>
       </c>
-      <c r="H14" s="71" t="str">
-        <f>'Tube K'!G11</f>
-        <v>F7</v>
-      </c>
-      <c r="I14" s="72">
-        <f>'Tube K'!F11</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="J14" s="73"/>
-      <c r="K14" s="71" t="str">
-        <f>'Tube L'!G11</f>
-        <v>E10</v>
-      </c>
-      <c r="L14" s="72">
-        <f>'Tube L'!F11</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="M14" s="73"/>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="58">
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="58">
         <v>11</v>
       </c>
-      <c r="B15" s="71" t="str">
+      <c r="B14" s="71" t="str">
         <f>'Tube I'!G12</f>
         <v>F2</v>
       </c>
-      <c r="C15" s="72">
+      <c r="C14" s="72">
         <f>'Tube I'!F12</f>
         <v>1.7130161300000015</v>
       </c>
-      <c r="D15" s="73">
+      <c r="D14" s="73">
         <v>5.8545983813505833</v>
       </c>
-      <c r="E15" s="71" t="str">
+      <c r="E14" s="71" t="str">
         <f>'Tube J'!G12</f>
         <v>A5</v>
       </c>
-      <c r="F15" s="69">
+      <c r="F14" s="69">
         <f>'Tube J'!F12</f>
         <v>1.7123058360000023</v>
       </c>
-      <c r="G15" s="73">
+      <c r="G14" s="73">
         <v>7.531650946019127</v>
       </c>
-      <c r="H15" s="71" t="str">
-        <f>'Tube K'!G12</f>
-        <v>G7</v>
-      </c>
-      <c r="I15" s="72">
-        <f>'Tube K'!F12</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="J15" s="73"/>
-      <c r="K15" s="71" t="str">
-        <f>'Tube L'!G12</f>
-        <v>D10</v>
-      </c>
-      <c r="L15" s="72">
-        <f>'Tube L'!F12</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="M15" s="75"/>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="58">
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="58">
         <v>12</v>
       </c>
-      <c r="B16" s="101" t="str">
+      <c r="B15" s="90" t="str">
         <f>'Tube I'!G13</f>
         <v>E2</v>
       </c>
-      <c r="C16" s="102">
+      <c r="C15" s="91">
         <f>'Tube I'!F13</f>
         <v>1.7064595700000016</v>
       </c>
-      <c r="D16" s="103">
+      <c r="D15" s="92">
         <v>3.7836760720548379</v>
       </c>
-      <c r="E16" s="71" t="str">
+      <c r="E15" s="71" t="str">
         <f>'Tube J'!G13</f>
         <v>B5</v>
       </c>
-      <c r="F16" s="69">
+      <c r="F15" s="69">
         <f>'Tube J'!F13</f>
         <v>1.7068420360000012</v>
       </c>
-      <c r="G16" s="73">
+      <c r="G15" s="73">
         <v>4.8121457945888046</v>
       </c>
-      <c r="H16" s="71" t="str">
-        <f>'Tube K'!G13</f>
-        <v>H7</v>
-      </c>
-      <c r="I16" s="72">
-        <f>'Tube K'!F13</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="J16" s="73"/>
-      <c r="K16" s="71" t="str">
-        <f>'Tube L'!G13</f>
-        <v>C10</v>
-      </c>
-      <c r="L16" s="72">
-        <f>'Tube L'!F13</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="M16" s="75"/>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="58">
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="58">
         <v>13</v>
       </c>
-      <c r="B17" s="71" t="str">
+      <c r="B16" s="71" t="str">
         <f>'Tube I'!G14</f>
         <v>D2</v>
       </c>
-      <c r="C17" s="72">
+      <c r="C16" s="72">
         <f>'Tube I'!F14</f>
         <v>1.7009957700000005</v>
       </c>
-      <c r="D17" s="73">
+      <c r="D16" s="73">
         <v>1.1063151421894843</v>
       </c>
-      <c r="E17" s="71" t="str">
+      <c r="E16" s="71" t="str">
         <f>'Tube J'!G14</f>
         <v>C5</v>
       </c>
-      <c r="F17" s="69">
+      <c r="F16" s="69">
         <f>'Tube J'!F14</f>
         <v>1.7015694690000007</v>
       </c>
-      <c r="G17" s="73">
+      <c r="G16" s="73">
         <v>1.5787694214818373</v>
       </c>
-      <c r="H17" s="71" t="str">
-        <f>'Tube K'!G14</f>
-        <v>H8</v>
-      </c>
-      <c r="I17" s="72">
-        <f>'Tube K'!F14</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="J17" s="73"/>
-      <c r="K17" s="71" t="str">
-        <f>'Tube L'!G14</f>
-        <v>B10</v>
-      </c>
-      <c r="L17" s="72">
-        <f>'Tube L'!F14</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="M17" s="75"/>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="58">
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="58">
         <v>14</v>
       </c>
-      <c r="B18" s="71" t="str">
+      <c r="B17" s="71" t="str">
         <f>'Tube I'!G15</f>
         <v>C2</v>
       </c>
-      <c r="C18" s="72">
+      <c r="C17" s="72">
         <f>'Tube I'!F15</f>
         <v>1.6946304430000012</v>
       </c>
-      <c r="D18" s="73">
+      <c r="D17" s="73">
         <v>0.54108544181554574</v>
       </c>
-      <c r="E18" s="71" t="str">
+      <c r="E17" s="71" t="str">
         <f>'Tube J'!G15</f>
         <v>D5</v>
       </c>
-      <c r="F18" s="69">
+      <c r="F17" s="69">
         <f>'Tube J'!F15</f>
         <v>1.6961056690000014</v>
       </c>
-      <c r="G18" s="73">
+      <c r="G17" s="73">
         <v>0.58025555929783046</v>
       </c>
-      <c r="H18" s="71" t="str">
-        <f>'Tube K'!G15</f>
-        <v>G8</v>
-      </c>
-      <c r="I18" s="72">
-        <f>'Tube K'!F15</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="J18" s="73"/>
-      <c r="K18" s="71" t="str">
-        <f>'Tube L'!G15</f>
-        <v>A10</v>
-      </c>
-      <c r="L18" s="72">
-        <f>'Tube L'!F15</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="M18" s="73"/>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="58">
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="58">
         <v>15</v>
       </c>
-      <c r="B19" s="71" t="str">
+      <c r="B18" s="71" t="str">
         <f>'Tube I'!G16</f>
         <v>B2</v>
       </c>
-      <c r="C19" s="72">
+      <c r="C18" s="72">
         <f>'Tube I'!F16</f>
         <v>1.6891666430000019</v>
       </c>
-      <c r="D19" s="73">
+      <c r="D18" s="73">
         <v>0.36896720819296275</v>
       </c>
-      <c r="E19" s="71" t="str">
+      <c r="E18" s="71" t="str">
         <f>'Tube J'!G16</f>
         <v>E5</v>
       </c>
-      <c r="F19" s="69">
+      <c r="F18" s="69">
         <f>'Tube J'!F16</f>
         <v>1.6895491090000014</v>
       </c>
-      <c r="G19" s="73">
+      <c r="G18" s="73">
         <v>0.29660628430541619</v>
       </c>
-      <c r="H19" s="71" t="str">
-        <f>'Tube K'!G16</f>
-        <v>F8</v>
-      </c>
-      <c r="I19" s="72">
-        <f>'Tube K'!F16</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="J19" s="73"/>
-      <c r="K19" s="71" t="str">
-        <f>'Tube L'!G16</f>
-        <v>A11</v>
-      </c>
-      <c r="L19" s="72">
-        <f>'Tube L'!F16</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="M19" s="73"/>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="58">
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="58">
         <v>16</v>
       </c>
-      <c r="B20" s="71" t="str">
+      <c r="B19" s="71" t="str">
         <f>'Tube I'!G17</f>
         <v>A2</v>
       </c>
-      <c r="C20" s="72">
+      <c r="C19" s="72">
         <f>'Tube I'!F17</f>
         <v>1.6826100830000019</v>
       </c>
-      <c r="D20" s="73">
+      <c r="D19" s="73">
         <v>0.15891702454462567</v>
       </c>
-      <c r="E20" s="71" t="str">
+      <c r="E19" s="71" t="str">
         <f>'Tube J'!G17</f>
         <v>F5</v>
       </c>
-      <c r="F20" s="69">
+      <c r="F19" s="69">
         <f>'Tube J'!F17</f>
         <v>1.6840853090000021</v>
       </c>
-      <c r="G20" s="73">
+      <c r="G19" s="73">
         <v>0.16316138281301762</v>
       </c>
-      <c r="H20" s="71" t="str">
-        <f>'Tube K'!G17</f>
-        <v>E8</v>
-      </c>
-      <c r="I20" s="72">
-        <f>'Tube K'!F17</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="J20" s="73"/>
-      <c r="K20" s="71" t="str">
-        <f>'Tube L'!G17</f>
-        <v>B11</v>
-      </c>
-      <c r="L20" s="72">
-        <f>'Tube L'!F17</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="M20" s="73"/>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="58">
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="58">
         <v>17</v>
       </c>
-      <c r="B21" s="71" t="str">
+      <c r="B20" s="71" t="str">
         <f>'Tube I'!G18</f>
         <v>A3</v>
       </c>
-      <c r="C21" s="72">
+      <c r="C20" s="72">
         <f>'Tube I'!F18</f>
         <v>1.6771462830000008</v>
       </c>
-      <c r="D21" s="73">
+      <c r="D20" s="73">
         <v>7.2987819654972849E-2</v>
       </c>
-      <c r="E21" s="71" t="str">
+      <c r="E20" s="71" t="str">
         <f>'Tube J'!G18</f>
         <v>G5</v>
       </c>
-      <c r="F21" s="69">
+      <c r="F20" s="69">
         <f>'Tube J'!F18</f>
         <v>1.6775287490000004</v>
       </c>
-      <c r="G21" s="73">
+      <c r="G20" s="73">
         <v>9.1546021857669843E-2</v>
       </c>
-      <c r="H21" s="71" t="str">
-        <f>'Tube K'!G18</f>
-        <v>D8</v>
-      </c>
-      <c r="I21" s="72">
-        <f>'Tube K'!F18</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="J21" s="73"/>
-      <c r="K21" s="71" t="str">
-        <f>'Tube L'!G18</f>
-        <v>C11</v>
-      </c>
-      <c r="L21" s="72">
-        <f>'Tube L'!F18</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="M21" s="73"/>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="58">
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="58">
         <v>18</v>
       </c>
-      <c r="B22" s="71" t="str">
+      <c r="B21" s="71" t="str">
         <f>'Tube I'!G19</f>
         <v>B3</v>
       </c>
-      <c r="C22" s="72">
+      <c r="C21" s="72">
         <f>'Tube I'!F19</f>
         <v>1.6694969630000021</v>
       </c>
-      <c r="D22" s="73">
+      <c r="D21" s="73">
         <v>6.5119570867859425E-2</v>
       </c>
-      <c r="E22" s="71" t="str">
+      <c r="E21" s="71" t="str">
         <f>'Tube J'!G19</f>
         <v>H5</v>
       </c>
-      <c r="F22" s="69">
+      <c r="F21" s="69">
         <f>'Tube J'!F19</f>
         <v>1.6698794290000016</v>
       </c>
-      <c r="G22" s="73">
+      <c r="G21" s="73">
         <v>7.9177263720196178E-2</v>
       </c>
-      <c r="H22" s="71" t="str">
-        <f>'Tube K'!G19</f>
-        <v>C8</v>
-      </c>
-      <c r="I22" s="72">
-        <f>'Tube K'!F19</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="J22" s="73"/>
-      <c r="K22" s="71" t="str">
-        <f>'Tube L'!G19</f>
-        <v>D11</v>
-      </c>
-      <c r="L22" s="72">
-        <f>'Tube L'!F19</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="M22" s="73"/>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="58">
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="58">
         <v>19</v>
       </c>
-      <c r="B23" s="71" t="str">
+      <c r="B22" s="71" t="str">
         <f>'Tube I'!G20</f>
         <v>C3</v>
       </c>
-      <c r="C23" s="72">
+      <c r="C22" s="72">
         <f>'Tube I'!F20</f>
         <v>1.6476417630000011</v>
       </c>
-      <c r="D23" s="73">
+      <c r="D22" s="73">
         <v>8.6478042616460485E-2</v>
       </c>
-      <c r="E23" s="71" t="str">
+      <c r="E22" s="71" t="str">
         <f>'Tube J'!G20</f>
         <v>H6</v>
       </c>
-      <c r="F23" s="69">
+      <c r="F22" s="69">
         <f>'Tube J'!F20</f>
         <v>1.6447459490000025</v>
       </c>
-      <c r="G23" s="73">
+      <c r="G22" s="73">
         <v>0.14114301618506389</v>
       </c>
-      <c r="H23" s="71" t="str">
-        <f>'Tube K'!G20</f>
-        <v>B8</v>
-      </c>
-      <c r="I23" s="72">
-        <f>'Tube K'!F20</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="J23" s="73"/>
-      <c r="K23" s="71" t="str">
-        <f>'Tube L'!G20</f>
-        <v>E11</v>
-      </c>
-      <c r="L23" s="72">
-        <f>'Tube L'!F20</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="M23" s="73"/>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="A24" s="58">
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="58">
         <v>20</v>
       </c>
-      <c r="B24" s="71" t="str">
+      <c r="B23" s="71" t="str">
         <f>'Tube I'!G21</f>
         <v>D3</v>
       </c>
-      <c r="C24" s="72">
+      <c r="C23" s="72">
         <f>'Tube I'!F21</f>
         <v>1.5634992430000008</v>
       </c>
-      <c r="D24" s="73">
+      <c r="D23" s="73">
         <v>6.5524490379192127E-2</v>
       </c>
-      <c r="E24" s="71" t="str">
+      <c r="E23" s="71" t="str">
         <f>'Tube J'!G21</f>
         <v>G6</v>
       </c>
-      <c r="F24" s="69">
+      <c r="F23" s="69">
         <f>'Tube J'!F21</f>
         <v>1.555139629000001</v>
       </c>
-      <c r="G24" s="73">
+      <c r="G23" s="73">
         <v>0.12154774185790913</v>
       </c>
-      <c r="H24" s="71" t="str">
-        <f>'Tube K'!G21</f>
-        <v>A8</v>
-      </c>
-      <c r="I24" s="72">
-        <f>'Tube K'!F21</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="J24" s="73"/>
-      <c r="K24" s="71" t="str">
-        <f>'Tube L'!G21</f>
-        <v>F11</v>
-      </c>
-      <c r="L24" s="72">
-        <f>'Tube L'!F21</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="M24" s="73"/>
-    </row>
-    <row r="25" spans="1:13">
-      <c r="A25" s="58">
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="58">
         <v>21</v>
       </c>
-      <c r="B25" s="104" t="str">
+      <c r="B24" s="93" t="str">
         <f>'Tube I'!G22</f>
         <v>E3</v>
       </c>
-      <c r="C25" s="105">
+      <c r="C24" s="94">
         <f>'Tube I'!F22</f>
         <v>1.382101083000002</v>
       </c>
-      <c r="D25" s="106">
+      <c r="D24" s="95">
         <v>5.0761947508031917E-2</v>
       </c>
-      <c r="E25" s="68" t="str">
+      <c r="E24" s="68" t="str">
         <f>'Tube J'!G22</f>
         <v>F6</v>
       </c>
-      <c r="F25" s="69">
+      <c r="F24" s="69">
         <f>'Tube J'!F22</f>
         <v>1.3748342290000028</v>
       </c>
-      <c r="G25" s="70">
+      <c r="G24" s="70">
         <v>6.8165058891525729E-2</v>
       </c>
-      <c r="H25" s="68" t="str">
-        <f>'Tube K'!G22</f>
-        <v>A9</v>
-      </c>
-      <c r="I25" s="69">
-        <f>'Tube K'!F22</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="J25" s="70"/>
-      <c r="K25" s="68" t="str">
-        <f>'Tube L'!G22</f>
-        <v>G11</v>
-      </c>
-      <c r="L25" s="69">
-        <f>'Tube L'!F22</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="M25" s="70"/>
-    </row>
-    <row r="26" spans="1:13" ht="13" thickBot="1">
-      <c r="A26" s="58">
+    </row>
+    <row r="25" spans="1:7" ht="13" thickBot="1">
+      <c r="A25" s="58">
         <v>22</v>
       </c>
-      <c r="B26" s="68" t="str">
+      <c r="B25" s="68" t="str">
         <f>'Tube I'!G23</f>
         <v>F3</v>
       </c>
-      <c r="C26" s="69">
+      <c r="C25" s="69">
         <f>'Tube I'!F23</f>
         <v>1.1646418430000018</v>
       </c>
-      <c r="D26" s="81">
+      <c r="D25" s="78">
         <v>2.8717598204228173E-2</v>
       </c>
-      <c r="E26" s="82" t="str">
+      <c r="E25" s="79" t="str">
         <f>'Tube J'!G23</f>
         <v>E6</v>
       </c>
-      <c r="F26" s="69">
+      <c r="F25" s="69">
         <f>'Tube J'!F23</f>
         <v>1.1650243090000014</v>
       </c>
-      <c r="G26" s="70">
+      <c r="G25" s="70">
         <v>2.8222377088385375E-2</v>
       </c>
-      <c r="H26" s="82" t="str">
-        <f>'Tube K'!G23</f>
-        <v>B9</v>
-      </c>
-      <c r="I26" s="83">
-        <f>'Tube K'!F23</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="J26" s="70"/>
-      <c r="K26" s="68" t="str">
-        <f>'Tube L'!G23</f>
-        <v>H11</v>
-      </c>
-      <c r="L26" s="83">
-        <f>'Tube L'!F23</f>
-        <v>-13.63998868</v>
-      </c>
-      <c r="M26" s="70"/>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="B27" s="84"/>
-      <c r="C27" s="85" t="s">
+    </row>
+    <row r="26" spans="1:7">
+      <c r="B26" s="80"/>
+      <c r="C26" s="81" t="s">
         <v>182</v>
       </c>
-      <c r="D27" s="77">
-        <f>SUM(D6:D26)*40/'Tube Loading'!J37*100</f>
+      <c r="D26" s="74">
+        <f>SUM(D5:D25)*40/'Tube Loading'!J37*100</f>
         <v>49.08513751382133</v>
       </c>
-      <c r="E27" s="72"/>
-      <c r="F27" s="85" t="s">
+      <c r="E26" s="72"/>
+      <c r="F26" s="81" t="s">
         <v>182</v>
       </c>
-      <c r="G27" s="86">
-        <f>SUM(G6:G26)*40/'Tube Loading'!J38*100</f>
+      <c r="G26" s="82">
+        <f>SUM(G5:G25)*40/'Tube Loading'!J38*100</f>
         <v>48.639814384326741</v>
       </c>
-      <c r="H27" s="72"/>
-      <c r="I27" s="76" t="s">
-        <v>182</v>
-      </c>
-      <c r="J27" s="86" t="e">
-        <f>SUM(J6:J26)*40/'Tube Loading'!J39*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K27" s="87"/>
-      <c r="L27" s="76" t="s">
-        <v>182</v>
-      </c>
-      <c r="M27" s="86" t="e">
-        <f>SUM(M6:M26)*40/'Tube Loading'!J40*100</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
+    </row>
+    <row r="28" spans="1:7">
       <c r="B28" s="72"/>
       <c r="C28" s="72"/>
       <c r="D28" s="72"/>
       <c r="E28" s="72"/>
       <c r="F28" s="72"/>
       <c r="G28" s="72"/>
-      <c r="H28" s="72"/>
-      <c r="I28" s="72"/>
-      <c r="J28" s="72"/>
-      <c r="K28" s="72"/>
-      <c r="L28" s="72"/>
-      <c r="M28" s="72"/>
-    </row>
-    <row r="29" spans="1:13">
+    </row>
+    <row r="29" spans="1:7">
       <c r="B29" s="72"/>
       <c r="C29" s="72"/>
       <c r="D29" s="72"/>
       <c r="E29" s="72"/>
       <c r="F29" s="72"/>
       <c r="G29" s="72"/>
-      <c r="H29" s="72"/>
-      <c r="I29" s="72"/>
-      <c r="J29" s="72"/>
-      <c r="K29" s="72"/>
-      <c r="L29" s="72"/>
-      <c r="M29" s="72"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="2">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="K3:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13986,19 +13484,19 @@
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="12.7"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="17.87890625" customWidth="1"/>
-    <col min="2" max="2" width="8.87890625" customWidth="1"/>
-    <col min="3" max="3" width="87.1171875" customWidth="1"/>
+    <col min="1" max="1" width="17.90625" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" customWidth="1"/>
+    <col min="3" max="3" width="87.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="13">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="50.7">
+    <row r="2" spans="1:6" ht="50">
       <c r="E2" s="2" t="s">
         <v>32</v>
       </c>
@@ -14040,7 +13538,7 @@
         <v>1550000000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.35">
+    <row r="5" spans="1:6" ht="15.5">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -14058,7 +13556,7 @@
         <v>1330000000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.35">
+    <row r="6" spans="1:6" ht="15.5">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
@@ -14075,7 +13573,7 @@
         <v>1220000000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.35">
+    <row r="7" spans="1:6" ht="15.5">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
@@ -14093,7 +13591,7 @@
         <v>1170000000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.35">
+    <row r="8" spans="1:6" ht="15.5">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -14110,7 +13608,7 @@
         <v>1140000000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.35">
+    <row r="9" spans="1:6" ht="15.5">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -14146,7 +13644,7 @@
         <v>1120000000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.35">
+    <row r="11" spans="1:6" ht="15.5">
       <c r="A11" s="3" t="s">
         <v>37</v>
       </c>
@@ -14213,11 +13711,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.35">
+    <row r="17" spans="1:4" ht="15.5">
       <c r="A17" s="3"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:4" ht="15.35">
+    <row r="18" spans="1:4" ht="15.5">
       <c r="C18" s="11" t="s">
         <v>38</v>
       </c>
@@ -14226,7 +13724,7 @@
         <v>19.166399999999982</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.35">
+    <row r="19" spans="1:4" ht="15.5">
       <c r="C19" s="11" t="s">
         <v>2</v>
       </c>
@@ -14235,7 +13733,7 @@
         <v>2.1295999999999977</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.35">
+    <row r="20" spans="1:4" ht="15.5">
       <c r="C20" s="11" t="s">
         <v>3</v>
       </c>
@@ -14244,126 +13742,126 @@
         <v>108.31629022640612</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.35">
+    <row r="22" spans="1:4" ht="15.5">
       <c r="C22" s="11"/>
       <c r="D22" s="12"/>
     </row>
-    <row r="23" spans="1:4" ht="15.35">
+    <row r="23" spans="1:4" ht="15.5">
       <c r="C23" s="11"/>
       <c r="D23" s="12"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" ht="13">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:4" ht="15.35">
+    <row r="28" spans="1:4" ht="15.5">
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:4" ht="15.35">
+    <row r="29" spans="1:4" ht="15.5">
       <c r="A29" s="3"/>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="1:4" ht="15.35">
+    <row r="30" spans="1:4" ht="15.5">
       <c r="A30" s="3"/>
       <c r="C30" s="4"/>
     </row>
-    <row r="31" spans="1:4" ht="15.35">
+    <row r="31" spans="1:4" ht="15.5">
       <c r="A31" s="3"/>
       <c r="B31" s="7"/>
       <c r="C31" s="4"/>
     </row>
-    <row r="32" spans="1:4" ht="15.35">
+    <row r="32" spans="1:4" ht="15.5">
       <c r="A32" s="3"/>
       <c r="C32" s="4"/>
     </row>
-    <row r="33" spans="1:12" ht="15.35">
+    <row r="33" spans="1:12" ht="15.5">
       <c r="A33" s="3"/>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:12" ht="15.35">
+    <row r="34" spans="1:12" ht="15.5">
       <c r="A34" s="3"/>
       <c r="C34" s="4"/>
     </row>
-    <row r="35" spans="1:12" ht="15.35">
+    <row r="35" spans="1:12" ht="15.5">
       <c r="A35" s="3"/>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:12" ht="15.35">
+    <row r="36" spans="1:12" ht="15.5">
       <c r="A36" s="3"/>
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="1:12" ht="15.35">
+    <row r="37" spans="1:12" ht="15.5">
       <c r="A37" s="3"/>
       <c r="B37" s="10"/>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:12" ht="15.35">
+    <row r="38" spans="1:12" ht="15.5">
       <c r="A38" s="3"/>
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="1:12" ht="15.35">
+    <row r="39" spans="1:12" ht="15.5">
       <c r="A39" s="3"/>
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:12" s="18" customFormat="1" ht="15.35">
+    <row r="40" spans="1:12" s="18" customFormat="1" ht="15.5">
       <c r="A40" s="17"/>
       <c r="C40" s="19"/>
     </row>
-    <row r="41" spans="1:12" ht="15.35">
+    <row r="41" spans="1:12" ht="15.5">
       <c r="A41" s="3"/>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:12" ht="15.35">
+    <row r="42" spans="1:12" ht="15.5">
       <c r="A42" s="3"/>
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:12" ht="15.35">
+    <row r="43" spans="1:12" ht="15.5">
       <c r="A43" s="3"/>
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:12" ht="15.35">
+    <row r="44" spans="1:12" ht="15.5">
       <c r="A44" s="3"/>
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="1:12" ht="15.35">
+    <row r="45" spans="1:12" ht="15.5">
       <c r="A45" s="3"/>
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:12" ht="15.35">
+    <row r="46" spans="1:12" ht="15.5">
       <c r="A46" s="3"/>
       <c r="C46" s="11"/>
     </row>
-    <row r="47" spans="1:12" ht="15.35">
+    <row r="47" spans="1:12" ht="15.5">
       <c r="C47" s="11"/>
       <c r="K47" s="20"/>
       <c r="L47" s="20"/>
     </row>
-    <row r="48" spans="1:12" ht="15.35">
+    <row r="48" spans="1:12" ht="15.5">
       <c r="C48" s="11"/>
     </row>
-    <row r="49" spans="3:12" s="20" customFormat="1" ht="15.35">
+    <row r="49" spans="3:12" s="20" customFormat="1" ht="15.5">
       <c r="C49" s="21"/>
       <c r="K49"/>
       <c r="L49"/>
     </row>
-    <row r="50" spans="3:12" ht="15.35">
+    <row r="50" spans="3:12" ht="15.5">
       <c r="C50" s="11"/>
     </row>
     <row r="51" spans="3:12">
       <c r="D51" s="13"/>
     </row>
-    <row r="52" spans="3:12" ht="15.35">
+    <row r="52" spans="3:12" ht="15.5">
       <c r="C52" s="11"/>
       <c r="D52" s="14"/>
     </row>
-    <row r="53" spans="3:12" ht="15.35">
+    <row r="53" spans="3:12" ht="15.5">
       <c r="C53" s="11"/>
       <c r="D53" s="14"/>
     </row>
-    <row r="54" spans="3:12" ht="15.35">
+    <row r="54" spans="3:12" ht="15.5">
       <c r="C54" s="11"/>
       <c r="D54" s="14"/>
     </row>
-    <row r="55" spans="3:12" ht="15.35">
+    <row r="55" spans="3:12" ht="15.5">
       <c r="C55" s="11"/>
     </row>
     <row r="56" spans="3:12">
@@ -14385,19 +13883,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.7"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="11.41015625" customWidth="1"/>
+    <col min="1" max="1" width="11.36328125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="12" width="11.41015625" customWidth="1"/>
-    <col min="13" max="13" width="12.29296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="11.36328125" customWidth="1"/>
+    <col min="13" max="13" width="12.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" ht="13">
       <c r="A1" s="3" t="s">
         <v>54</v>
       </c>
@@ -14466,7 +13964,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" ht="13">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
@@ -14559,7 +14057,7 @@
         <v>5.2630546676799987</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" ht="13">
       <c r="A19" s="31">
         <v>4.3</v>
       </c>
@@ -14801,7 +14299,7 @@
       <c r="B27" s="16"/>
       <c r="C27" s="30"/>
     </row>
-    <row r="28" spans="1:11" ht="38">
+    <row r="28" spans="1:11" ht="39">
       <c r="A28" s="40" t="s">
         <v>43</v>
       </c>
@@ -14833,7 +14331,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="13.7">
+    <row r="29" spans="1:11" ht="14">
       <c r="A29" t="s">
         <v>138</v>
       </c>
@@ -14847,7 +14345,7 @@
         <f t="shared" ref="E29:E40" si="6">D29*10.9276-13.593</f>
         <v>-13.631246600000001</v>
       </c>
-      <c r="F29" s="88"/>
+      <c r="F29" s="83"/>
       <c r="H29" s="52" t="e">
         <f>4000/G29</f>
         <v>#DIV/0!</v>
@@ -14857,11 +14355,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="J29" t="e">
-        <f t="shared" ref="J29:J35" si="7">G29*H29</f>
+        <f t="shared" ref="J29:J30" si="7">G29*H29</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="13.7">
+    <row r="30" spans="1:11" ht="14">
       <c r="A30" t="s">
         <v>139</v>
       </c>
@@ -14875,7 +14373,7 @@
         <f t="shared" si="6"/>
         <v>-13.631246600000001</v>
       </c>
-      <c r="F30" s="94"/>
+      <c r="F30" s="89"/>
       <c r="H30" s="52" t="e">
         <f>4000/G30</f>
         <v>#DIV/0!</v>
@@ -14889,7 +14387,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="13.7">
+    <row r="31" spans="1:11" ht="14">
       <c r="A31" t="s">
         <v>140</v>
       </c>
@@ -14903,7 +14401,7 @@
         <f t="shared" si="6"/>
         <v>-13.631246600000001</v>
       </c>
-      <c r="F31" s="88"/>
+      <c r="F31" s="83"/>
       <c r="H31" s="52" t="e">
         <f t="shared" ref="H31:H36" si="8">4000/G31</f>
         <v>#DIV/0!</v>
@@ -14917,7 +14415,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="13.7">
+    <row r="32" spans="1:11" ht="14">
       <c r="A32" t="s">
         <v>141</v>
       </c>
@@ -14931,7 +14429,7 @@
         <f t="shared" si="6"/>
         <v>-13.631246600000001</v>
       </c>
-      <c r="F32" s="93"/>
+      <c r="F32" s="88"/>
       <c r="H32" s="52" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -14945,7 +14443,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="13.7">
+    <row r="33" spans="1:10" ht="14">
       <c r="A33" t="s">
         <v>142</v>
       </c>
@@ -14959,7 +14457,7 @@
         <f t="shared" si="6"/>
         <v>-13.631246600000001</v>
       </c>
-      <c r="F33" s="93"/>
+      <c r="F33" s="88"/>
       <c r="H33" s="52" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -14987,7 +14485,7 @@
         <f t="shared" si="6"/>
         <v>-13.631246600000001</v>
       </c>
-      <c r="F34" s="90"/>
+      <c r="F34" s="85"/>
       <c r="H34" s="52" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -15001,7 +14499,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="13.7">
+    <row r="35" spans="1:10" ht="14">
       <c r="A35" t="s">
         <v>144</v>
       </c>
@@ -15015,7 +14513,7 @@
         <f t="shared" si="6"/>
         <v>-13.631246600000001</v>
       </c>
-      <c r="F35" s="88"/>
+      <c r="F35" s="83"/>
       <c r="H35" s="52" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -15029,7 +14527,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="13.7">
+    <row r="36" spans="1:10" ht="14">
       <c r="A36" t="s">
         <v>145</v>
       </c>
@@ -15043,7 +14541,7 @@
         <f t="shared" si="6"/>
         <v>-13.631246600000001</v>
       </c>
-      <c r="F36" s="93"/>
+      <c r="F36" s="88"/>
       <c r="H36" s="52" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -15057,7 +14555,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="13.7">
+    <row r="37" spans="1:10" ht="14">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -15075,7 +14573,7 @@
         <f t="shared" si="6"/>
         <v>1.7259380169999989</v>
       </c>
-      <c r="F37" s="88">
+      <c r="F37" s="83">
         <v>1454</v>
       </c>
       <c r="G37">
@@ -15086,7 +14584,7 @@
         <v>24.4299674267101</v>
       </c>
       <c r="I37" s="52">
-        <f t="shared" ref="I32:I42" si="11">150-H37</f>
+        <f t="shared" ref="I37:I42" si="11">150-H37</f>
         <v>125.57003257328989</v>
       </c>
       <c r="J37">
@@ -15094,7 +14592,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="13.7">
+    <row r="38" spans="1:10" ht="14">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -15112,7 +14610,7 @@
         <f t="shared" si="6"/>
         <v>1.7281235370000001</v>
       </c>
-      <c r="F38" s="88">
+      <c r="F38" s="83">
         <v>1469</v>
       </c>
       <c r="G38">
@@ -15127,11 +14625,11 @@
         <v>107.86516853932585</v>
       </c>
       <c r="J38">
-        <f t="shared" ref="J36:J44" si="12">G38*H38</f>
+        <f t="shared" ref="J38:J44" si="12">G38*H38</f>
         <v>3000</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="14.35">
+    <row r="39" spans="1:10" ht="14.5">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -15145,8 +14643,8 @@
         <f t="shared" si="6"/>
         <v>-13.631246600000001</v>
       </c>
-      <c r="F39" s="89"/>
-      <c r="G39" s="92"/>
+      <c r="F39" s="84"/>
+      <c r="G39" s="87"/>
       <c r="H39" s="52" t="e">
         <f>1000/G39</f>
         <v>#DIV/0!</v>
@@ -15160,7 +14658,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="13.7">
+    <row r="40" spans="1:10" ht="14">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -15174,7 +14672,7 @@
         <f t="shared" si="6"/>
         <v>-13.631246600000001</v>
       </c>
-      <c r="F40" s="91"/>
+      <c r="F40" s="86"/>
       <c r="H40" s="52" t="e">
         <f>4000/G40</f>
         <v>#DIV/0!</v>
@@ -15188,7 +14686,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="13.7">
+    <row r="41" spans="1:10" ht="14">
       <c r="A41" t="s">
         <v>163</v>
       </c>
@@ -15202,7 +14700,7 @@
         <f>D41*10.9276-13.593</f>
         <v>-13.631246600000001</v>
       </c>
-      <c r="F41" s="91"/>
+      <c r="F41" s="86"/>
       <c r="H41" s="52" t="e">
         <f>4000/G41</f>
         <v>#DIV/0!</v>
@@ -15216,7 +14714,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="13.7">
+    <row r="42" spans="1:10" ht="14">
       <c r="A42" t="s">
         <v>164</v>
       </c>
@@ -15230,7 +14728,7 @@
         <f>D42*10.9276-13.593</f>
         <v>-13.631246600000001</v>
       </c>
-      <c r="F42" s="91"/>
+      <c r="F42" s="86"/>
       <c r="H42" s="52" t="e">
         <f>4000/G42</f>
         <v>#DIV/0!</v>
@@ -15244,7 +14742,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="13.7">
+    <row r="43" spans="1:10" ht="14">
       <c r="A43" t="s">
         <v>165</v>
       </c>
@@ -15258,7 +14756,7 @@
         <f>D43*10.9276-13.593</f>
         <v>-13.631246600000001</v>
       </c>
-      <c r="F43" s="91"/>
+      <c r="F43" s="86"/>
       <c r="H43" s="52" t="e">
         <f>1000/G43</f>
         <v>#DIV/0!</v>
@@ -15272,7 +14770,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="13.7">
+    <row r="44" spans="1:10" ht="14">
       <c r="A44" t="s">
         <v>166</v>
       </c>
@@ -15286,7 +14784,7 @@
         <f>D44*10.9276-13.593</f>
         <v>-13.631246600000001</v>
       </c>
-      <c r="F44" s="91"/>
+      <c r="F44" s="86"/>
       <c r="H44" s="52" t="e">
         <f>1000/G44</f>
         <v>#DIV/0!</v>
@@ -15300,7 +14798,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="13.7">
+    <row r="45" spans="1:10" ht="14">
       <c r="A45" s="47" t="s">
         <v>33</v>
       </c>
@@ -15318,11 +14816,11 @@
         <f>D45*10.9276-13.593</f>
         <v>1.8868196079999997</v>
       </c>
-      <c r="F45" s="91"/>
+      <c r="F45" s="86"/>
       <c r="H45" s="52"/>
       <c r="I45" s="52"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" ht="13">
       <c r="B46" s="26"/>
       <c r="C46" s="23"/>
       <c r="F46" s="3"/>
@@ -15365,9 +14863,9 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.7"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.35">
+    <row r="1" spans="1:13" ht="26">
       <c r="A1" s="32" t="s">
         <v>55</v>
       </c>
@@ -15982,9 +15480,9 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.7"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.35">
+    <row r="1" spans="1:13" ht="26">
       <c r="A1" s="32" t="s">
         <v>55</v>
       </c>
@@ -16599,9 +16097,9 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.7"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.35">
+    <row r="1" spans="1:13" ht="26">
       <c r="A1" s="32" t="s">
         <v>55</v>
       </c>
@@ -17216,9 +16714,9 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.7"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.35">
+    <row r="1" spans="1:13" ht="26">
       <c r="A1" s="32" t="s">
         <v>55</v>
       </c>
@@ -17833,9 +17331,9 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.7"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.35">
+    <row r="1" spans="1:13" ht="26">
       <c r="A1" s="32" t="s">
         <v>55</v>
       </c>
@@ -18450,9 +17948,9 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.7"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.35">
+    <row r="1" spans="1:13" ht="26">
       <c r="A1" s="32" t="s">
         <v>55</v>
       </c>

</xml_diff>